<commit_message>
fix: change new template and fixing date picker filter
</commit_message>
<xml_diff>
--- a/public/template_excel/alat_pertanian.xlsx
+++ b/public/template_excel/alat_pertanian.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D42E148-3A9B-4663-A1C4-C8FF9D857A22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91C99E74-2286-4FC0-904A-B00F9988C067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1200" yWindow="-14790" windowWidth="24750" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="alat_pertanian" sheetId="2" r:id="rId1"/>
@@ -321,7 +321,9 @@
   </sheetPr>
   <dimension ref="A1:P731"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -367,7 +369,7 @@
     <row r="2" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
+      <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="3"/>

</xml_diff>